<commit_message>
Atualizado o Backlog e relatorio de acompanhamento
</commit_message>
<xml_diff>
--- a/documentacao/Backlog-do-produto.xlsx
+++ b/documentacao/Backlog-do-produto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20191134040017\Documents\IFRN\2021\2021.2\P.I - RH\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749A2CA3-1CD1-42D2-A4FA-46680AB64141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7818BA4E-9771-46B6-B08A-81EDD78F75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4485" windowWidth="20730" windowHeight="11040" xr2:uid="{27396E15-7517-4D93-B3B1-F514BB1226D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27396E15-7517-4D93-B3B1-F514BB1226D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,14 +197,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,11 +247,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -393,13 +380,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -410,12 +396,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="5" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,10 +421,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="20% - Ênfase3" xfId="5" builtinId="38"/>
+  <cellStyles count="5">
+    <cellStyle name="20% - Ênfase3" xfId="4" builtinId="38"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Cálculo" xfId="4" builtinId="22"/>
     <cellStyle name="Neutro" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Ruim" xfId="2" builtinId="27"/>
@@ -755,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C0FA35-851E-4E02-9249-2AF73D7C3452}">
   <dimension ref="E6:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M20" sqref="L20:M20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,8 +1068,8 @@
       <c r="L19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="12" t="s">
-        <v>24</v>
+      <c r="M19" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.25">
@@ -1106,8 +1091,8 @@
       <c r="L20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>24</v>
+      <c r="M20" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.25">
@@ -1278,7 +1263,7 @@
       <c r="M30" s="3"/>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="13"/>
+      <c r="K33" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>